<commit_message>
added error handling for array data in a cell
</commit_message>
<xml_diff>
--- a/mapping_v2.xlsx
+++ b/mapping_v2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Xchange\Studis\Apath\HiWi Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Xchange\Studis\Apath\HiWi Project-Industry\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E70902-716A-4C00-BF1E-DA9BEBFF148F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8148"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEDOS_parameters" sheetId="5" r:id="rId1"/>
@@ -26,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="278">
   <si>
     <t>TIMES</t>
   </si>
@@ -884,12 +885,15 @@
   </si>
   <si>
     <t>STG_CHRG</t>
+  </si>
+  <si>
+    <t>STG_MAXCYC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1100,8 +1104,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1515,27 +1519,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1567,7 +1571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>167</v>
       </c>
@@ -1578,7 +1582,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -1603,7 +1607,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -1624,7 +1628,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>54</v>
       </c>
@@ -1637,7 +1641,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1652,7 +1656,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>169</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>170</v>
       </c>
@@ -1686,7 +1690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>171</v>
       </c>
@@ -1700,7 +1704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
@@ -1711,7 +1715,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>172</v>
       </c>
@@ -1725,7 +1729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>173</v>
       </c>
@@ -1739,7 +1743,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>174</v>
       </c>
@@ -1764,7 +1768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>175</v>
       </c>
@@ -1778,7 +1782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>176</v>
       </c>
@@ -1789,7 +1793,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>83</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
@@ -1817,7 +1821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>70</v>
       </c>
@@ -1831,7 +1835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>177</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>178</v>
       </c>
@@ -1862,7 +1866,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="30" t="s">
         <v>179</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>84</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -1899,7 +1903,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>66</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>180</v>
       </c>
@@ -1921,7 +1925,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>86</v>
       </c>
@@ -1932,7 +1936,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>76</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>67</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>181</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -1976,7 +1980,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>182</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>183</v>
       </c>
@@ -2006,7 +2010,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>184</v>
       </c>
@@ -2020,7 +2024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>185</v>
       </c>
@@ -2034,7 +2038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>186</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>187</v>
       </c>
@@ -2059,7 +2063,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="30" t="s">
         <v>188</v>
       </c>
@@ -2071,7 +2075,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>189</v>
       </c>
@@ -2085,7 +2089,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>190</v>
       </c>
@@ -2096,7 +2100,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>191</v>
       </c>
@@ -2107,7 +2111,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
         <v>192</v>
       </c>
@@ -2116,7 +2120,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="22" t="s">
         <v>193</v>
       </c>
@@ -2127,7 +2131,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="22" t="s">
         <v>194</v>
       </c>
@@ -2138,7 +2142,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="22" t="s">
         <v>195</v>
       </c>
@@ -2147,7 +2151,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="22" t="s">
         <v>196</v>
       </c>
@@ -2156,16 +2160,18 @@
         <v>252</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="B51" s="22"/>
+      <c r="B51" s="22" t="s">
+        <v>277</v>
+      </c>
       <c r="C51" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="22" t="s">
         <v>198</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="22" t="s">
         <v>199</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>200</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="22" t="s">
         <v>201</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>202</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="23" t="s">
         <v>203</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="23" t="s">
         <v>204</v>
       </c>
@@ -2237,7 +2243,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="22" t="s">
         <v>205</v>
       </c>
@@ -2246,7 +2252,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="22" t="s">
         <v>206</v>
       </c>
@@ -2255,7 +2261,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="23" t="s">
         <v>207</v>
       </c>
@@ -2266,19 +2272,19 @@
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>208</v>
       </c>
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>209</v>
       </c>
       <c r="B63" s="6"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>210</v>
       </c>
@@ -2287,199 +2293,199 @@
         <v>264</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B65" s="6"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>211</v>
       </c>
       <c r="B66" s="6"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>212</v>
       </c>
       <c r="B67" s="6"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>213</v>
       </c>
       <c r="B68" s="6"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>214</v>
       </c>
       <c r="B69" s="6"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>215</v>
       </c>
       <c r="B70" s="6"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B71" s="6"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>216</v>
       </c>
       <c r="B72" s="6"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B73" s="6"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B74" s="6"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B75" s="6"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B76" s="6"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B77" s="6"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B78" s="6"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B79" s="6"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B80" s="6"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="6"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="6"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="6"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="6"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="6"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" s="6"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" s="6"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" s="6"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89" s="6"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" s="6"/>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B91" s="6"/>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B92" s="6"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B93" s="6"/>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B94" s="6"/>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B95" s="6"/>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B96" s="6"/>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B98" s="6"/>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B99" s="6"/>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B100" s="6"/>
     </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B101" s="6"/>
     </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B102" s="6"/>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B103" s="6"/>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B104" s="6"/>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B105" s="6"/>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B106" s="6"/>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B107" s="6"/>
     </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B108" s="6"/>
     </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B109" s="6"/>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B110" s="6"/>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B111" s="6"/>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B112" s="6"/>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B113" s="6"/>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B114" s="6"/>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B115" s="6"/>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B116" s="6"/>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B117" s="6"/>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B118" s="6"/>
     </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B119" s="6"/>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B120" s="6"/>
     </row>
   </sheetData>
@@ -2489,22 +2495,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -2518,7 +2524,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="31.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -2532,7 +2538,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -2543,7 +2549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>49</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>91</v>
       </c>
@@ -2559,7 +2565,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>91</v>
       </c>
@@ -2567,7 +2573,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>92</v>
       </c>
@@ -2575,7 +2581,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>92</v>
       </c>
@@ -2583,7 +2589,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>93</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>92</v>
       </c>
@@ -2599,7 +2605,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>94</v>
       </c>
@@ -2607,7 +2613,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>95</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>96</v>
       </c>
@@ -2623,7 +2629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>97</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>98</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>99</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>98</v>
       </c>
@@ -2655,7 +2661,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>100</v>
       </c>
@@ -2663,7 +2669,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>99</v>
       </c>
@@ -2671,7 +2677,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>101</v>
       </c>
@@ -2679,7 +2685,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>102</v>
       </c>
@@ -2687,7 +2693,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>103</v>
       </c>
@@ -2695,7 +2701,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>104</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>105</v>
       </c>
@@ -2711,7 +2717,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>106</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>107</v>
       </c>
@@ -2727,7 +2733,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>108</v>
       </c>
@@ -2735,7 +2741,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>109</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>50</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>97</v>
       </c>
@@ -2762,7 +2768,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>99</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>51</v>
       </c>
@@ -2781,7 +2787,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>94</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>52</v>
       </c>
@@ -2797,7 +2803,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
@@ -2805,7 +2811,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
         <v>110</v>
       </c>
@@ -2813,7 +2819,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>111</v>
       </c>
@@ -2821,7 +2827,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>112</v>
       </c>
@@ -2829,7 +2835,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>113</v>
       </c>
@@ -2837,7 +2843,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>114</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
         <v>115</v>
       </c>
@@ -2853,7 +2859,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>116</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="11" t="s">
         <v>117</v>
       </c>
@@ -2875,7 +2881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>118</v>
       </c>
@@ -2886,7 +2892,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
         <v>119</v>
       </c>
@@ -2897,7 +2903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
         <v>120</v>
       </c>
@@ -2908,7 +2914,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
         <v>121</v>
       </c>
@@ -2919,7 +2925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
         <v>122</v>
       </c>
@@ -2929,7 +2935,7 @@
       </c>
       <c r="D48" s="15"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
         <v>123</v>
       </c>
@@ -2939,7 +2945,7 @@
       </c>
       <c r="D49" s="15"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>124</v>
       </c>
@@ -2949,7 +2955,7 @@
       </c>
       <c r="D50" s="15"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>125</v>
       </c>
@@ -2959,7 +2965,7 @@
       </c>
       <c r="D51" s="15"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="14" t="s">
         <v>126</v>
       </c>
@@ -2969,7 +2975,7 @@
       </c>
       <c r="D52" s="15"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>127</v>
       </c>
@@ -2979,7 +2985,7 @@
       </c>
       <c r="D53" s="15"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="14" t="s">
         <v>128</v>
       </c>
@@ -2989,7 +2995,7 @@
       </c>
       <c r="D54" s="15"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="14" t="s">
         <v>129</v>
       </c>
@@ -2999,7 +3005,7 @@
       </c>
       <c r="D55" s="15"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>112</v>
       </c>
@@ -3011,7 +3017,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>130</v>
       </c>
@@ -3019,7 +3025,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
         <v>131</v>
       </c>
@@ -3030,7 +3036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="19" t="s">
         <v>132</v>
       </c>
@@ -3038,7 +3044,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>133</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="17" t="s">
         <v>134</v>
       </c>
@@ -3054,7 +3060,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="19" t="s">
         <v>135</v>
       </c>
@@ -3062,7 +3068,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="18" t="s">
         <v>136</v>
       </c>
@@ -3073,7 +3079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
         <v>137</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
         <v>138</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
         <v>139</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
         <v>140</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="18" t="s">
         <v>141</v>
       </c>
@@ -3113,7 +3119,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="18" t="s">
         <v>142</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="19" t="s">
         <v>143</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="19" t="s">
         <v>91</v>
       </c>
@@ -3137,7 +3143,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="18" t="s">
         <v>144</v>
       </c>
@@ -3148,7 +3154,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="20" t="s">
         <v>91</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="18" t="s">
         <v>92</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="18" t="s">
         <v>92</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="19" t="s">
         <v>145</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="18" t="s">
         <v>146</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="18" t="s">
         <v>147</v>
       </c>
@@ -3199,7 +3205,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="18" t="s">
         <v>94</v>
       </c>
@@ -3207,7 +3213,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="18" t="s">
         <v>96</v>
       </c>
@@ -3215,7 +3221,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="18" t="s">
         <v>148</v>
       </c>
@@ -3223,7 +3229,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="18" t="s">
         <v>97</v>
       </c>
@@ -3231,7 +3237,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="18" t="s">
         <v>98</v>
       </c>
@@ -3239,7 +3245,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="18" t="s">
         <v>99</v>
       </c>
@@ -3247,7 +3253,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="18" t="s">
         <v>98</v>
       </c>
@@ -3255,7 +3261,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="18" t="s">
         <v>100</v>
       </c>
@@ -3263,7 +3269,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="18" t="s">
         <v>102</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="18" t="s">
         <v>149</v>
       </c>
@@ -3282,7 +3288,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="18" t="s">
         <v>150</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="18" t="s">
         <v>151</v>
       </c>
@@ -3298,7 +3304,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="18" t="s">
         <v>109</v>
       </c>
@@ -3306,7 +3312,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="18" t="s">
         <v>152</v>
       </c>
@@ -3314,7 +3320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="18" t="s">
         <v>153</v>
       </c>
@@ -3322,7 +3328,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="18" t="s">
         <v>99</v>
       </c>
@@ -3330,7 +3336,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="18" t="s">
         <v>154</v>
       </c>
@@ -3338,7 +3344,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="18" t="s">
         <v>155</v>
       </c>
@@ -3346,7 +3352,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="18" t="s">
         <v>116</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="18" t="s">
         <v>156</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="18" t="s">
         <v>93</v>
       </c>
@@ -3370,7 +3376,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="18" t="s">
         <v>157</v>
       </c>
@@ -3381,7 +3387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="18" t="s">
         <v>158</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="19" t="s">
         <v>159</v>
       </c>
@@ -3403,7 +3409,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="19" t="s">
         <v>160</v>
       </c>
@@ -3414,7 +3420,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="18" t="s">
         <v>161</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="18" t="s">
         <v>162</v>
       </c>
@@ -3436,7 +3442,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="18" t="s">
         <v>163</v>
       </c>
@@ -3447,7 +3453,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="17" t="s">
         <v>164</v>
       </c>
@@ -3455,7 +3461,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="17" t="s">
         <v>164</v>
       </c>
@@ -3463,7 +3469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="18" t="s">
         <v>164</v>
       </c>
@@ -3471,7 +3477,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="19" t="s">
         <v>165</v>
       </c>
@@ -3482,7 +3488,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="19" t="s">
         <v>166</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="26" t="s">
         <v>267</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="26" t="s">
         <v>164</v>
       </c>
@@ -3509,7 +3515,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="26" t="s">
         <v>156</v>
       </c>
@@ -3517,7 +3523,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="26" t="s">
         <v>268</v>
       </c>
@@ -3528,7 +3534,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="27" t="s">
         <v>37</v>
       </c>
@@ -3539,7 +3545,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="26" t="s">
         <v>41</v>
       </c>
@@ -3550,7 +3556,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="26" t="s">
         <v>40</v>
       </c>
@@ -3561,7 +3567,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="26" t="s">
         <v>39</v>
       </c>
@@ -3572,7 +3578,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="26" t="s">
         <v>35</v>
       </c>
@@ -3583,7 +3589,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="26" t="s">
         <v>38</v>
       </c>
@@ -3602,16 +3608,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3622,7 +3628,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -3630,7 +3636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3638,7 +3644,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>

</xml_diff>